<commit_message>
updated templates for Scores
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionBook/Scores-A4.xlsx
+++ b/owlcms/src/main/resources/templates/competitionBook/Scores-A4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7D8FFE-98A1-48B3-A7E8-E8C1CEDB0DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8C82B7-8C47-448B-8DEB-31C44A84EE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="447" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="4065" windowWidth="23205" windowHeight="11295" tabRatio="447" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="35" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="148">
   <si>
     <t>${l.lastName}</t>
   </si>
@@ -491,6 +491,9 @@
   </si>
   <si>
     <t>&lt;jx:forEach items="${wCus}" groupBy="category.code"&gt;</t>
+  </si>
+  <si>
+    <t>${t.get("Category")}</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1182,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1426,13 +1429,7 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1458,6 +1455,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1513,10 +1514,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2200,14 +2197,14 @@
       <c r="A1" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
       <c r="J1" s="39" t="s">
@@ -2221,14 +2218,14 @@
       <c r="A2" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
       <c r="J2" s="39" t="s">
@@ -2242,14 +2239,14 @@
       <c r="A3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="103" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
       <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -3876,7 +3873,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="91" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="86" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -4231,7 +4228,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="79" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="74" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -4250,7 +4247,7 @@
   <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4482,7 +4479,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="60" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -6122,7 +6119,7 @@
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -6135,7 +6132,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X107"/>
+  <dimension ref="A1:Z107"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A2"/>
@@ -6163,63 +6160,69 @@
     <col min="18" max="18" width="6.28515625" style="1" customWidth="1"/>
     <col min="19" max="20" width="6.28515625" customWidth="1"/>
     <col min="21" max="21" width="6.85546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="1" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="110" t="s">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="118" t="s">
+      <c r="F1" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="118" t="s">
+      <c r="H1" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="120" t="s">
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="106" t="s">
-        <v>102</v>
-      </c>
-      <c r="T1" s="107"/>
-      <c r="U1" s="108"/>
-    </row>
-    <row r="2" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="111"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="105" t="s">
+        <v>147</v>
+      </c>
+      <c r="T1" s="106"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="104" t="s">
+        <v>144</v>
+      </c>
+      <c r="W1" s="104"/>
+    </row>
+    <row r="2" spans="1:26" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="110"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
       <c r="I2" s="32">
         <v>1</v>
       </c>
@@ -6259,8 +6262,14 @@
       <c r="U2" s="51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V2" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="W2" s="51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="52" t="s">
         <v>145</v>
       </c>
@@ -6275,7 +6284,7 @@
       <c r="J3" s="54"/>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:24" s="18" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" s="18" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="53"/>
       <c r="B4" s="53"/>
       <c r="C4" s="53"/>
@@ -6288,7 +6297,7 @@
       <c r="J4" s="54"/>
       <c r="K4" s="55"/>
     </row>
-    <row r="5" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="56" t="s">
         <v>92</v>
       </c>
@@ -6312,11 +6321,13 @@
       <c r="S5" s="58"/>
       <c r="T5" s="58"/>
       <c r="U5" s="59"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="59"/>
       <c r="X5" s="1"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -6335,8 +6346,9 @@
       <c r="Q6"/>
       <c r="R6"/>
       <c r="U6"/>
-    </row>
-    <row r="7" spans="1:24" s="18" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W6"/>
+    </row>
+    <row r="7" spans="1:26" s="18" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>19</v>
       </c>
@@ -6398,8 +6410,14 @@
       <c r="U7" s="49" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="V7" s="99" t="s">
+        <v>142</v>
+      </c>
+      <c r="W7" s="100" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -6417,8 +6435,9 @@
       <c r="Q8"/>
       <c r="R8"/>
       <c r="U8"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W8"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -6436,30 +6455,31 @@
       <c r="Q9"/>
       <c r="R9"/>
       <c r="U9"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W9"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B13" s="19"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
-      <c r="R15" s="109"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R15" s="108"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
-      <c r="R16" s="109"/>
+      <c r="R16" s="108"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
@@ -6736,7 +6756,8 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="V1:W1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="R15:R16"/>
     <mergeCell ref="A1:A2"/>
@@ -6780,7 +6801,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="81" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -6793,7 +6814,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W108"/>
+  <dimension ref="A1:Y108"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:A2"/>
@@ -6821,62 +6842,68 @@
     <col min="18" max="18" width="6.28515625" style="1" customWidth="1"/>
     <col min="19" max="20" width="6.28515625" customWidth="1"/>
     <col min="21" max="21" width="6.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="110" t="s">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="118" t="s">
+      <c r="F1" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="118" t="s">
+      <c r="H1" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="120" t="s">
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="106" t="s">
-        <v>102</v>
-      </c>
-      <c r="T1" s="107"/>
-      <c r="U1" s="108"/>
-    </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="111"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="105" t="s">
+        <v>147</v>
+      </c>
+      <c r="T1" s="106"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="104" t="s">
+        <v>144</v>
+      </c>
+      <c r="W1" s="104"/>
+    </row>
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="110"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
       <c r="I2" s="32">
         <v>1</v>
       </c>
@@ -6916,8 +6943,14 @@
       <c r="U2" s="51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V2" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="W2" s="51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="52" t="s">
         <v>146</v>
       </c>
@@ -6932,7 +6965,7 @@
       <c r="J3" s="54"/>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:23" s="18" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="18" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="53"/>
       <c r="B4" s="53"/>
       <c r="C4" s="53"/>
@@ -6945,7 +6978,7 @@
       <c r="J4" s="54"/>
       <c r="K4" s="55"/>
     </row>
-    <row r="5" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="56" t="s">
         <v>92</v>
       </c>
@@ -6969,10 +7002,12 @@
       <c r="S5" s="58"/>
       <c r="T5" s="58"/>
       <c r="U5" s="59"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V5" s="58"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -6990,8 +7025,9 @@
       <c r="P6"/>
       <c r="R6"/>
       <c r="U6"/>
-    </row>
-    <row r="7" spans="1:23" s="18" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W6"/>
+    </row>
+    <row r="7" spans="1:25" s="18" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>19</v>
       </c>
@@ -7053,8 +7089,14 @@
       <c r="U7" s="49" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V7" s="99" t="s">
+        <v>142</v>
+      </c>
+      <c r="W7" s="100" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -7072,8 +7114,9 @@
       <c r="P8"/>
       <c r="R8"/>
       <c r="U8"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W8"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -7091,33 +7134,34 @@
       <c r="P9"/>
       <c r="R9"/>
       <c r="U9"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W9"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B14" s="19"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
-      <c r="P16" s="109"/>
+      <c r="P16" s="108"/>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
-      <c r="P17" s="109"/>
+      <c r="P17" s="108"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C18" s="1"/>
@@ -7394,7 +7438,8 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="V1:W1"/>
     <mergeCell ref="P16:P17"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="A1:A2"/>
@@ -7438,7 +7483,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="82" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="77" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -7483,58 +7528,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="118" t="s">
+      <c r="F1" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="118" t="s">
+      <c r="H1" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="120" t="s">
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="106" t="s">
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="108"/>
+      <c r="T1" s="107"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="111"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
       <c r="I2" s="32">
         <v>1</v>
       </c>
@@ -7763,11 +7808,11 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
-      <c r="R15" s="109"/>
+      <c r="R15" s="108"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
-      <c r="R16" s="109"/>
+      <c r="R16" s="108"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
@@ -8088,7 +8133,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="84" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="79" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -8132,58 +8177,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="118" t="s">
+      <c r="F1" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="118" t="s">
+      <c r="H1" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="120" t="s">
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="106" t="s">
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="108"/>
+      <c r="T1" s="107"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="111"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
       <c r="I2" s="32">
         <v>1</v>
       </c>
@@ -8411,11 +8456,11 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
-      <c r="P16" s="109"/>
+      <c r="P16" s="108"/>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
-      <c r="P17" s="109"/>
+      <c r="P17" s="108"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C18" s="1"/>
@@ -8736,7 +8781,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="85" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="79" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -8769,69 +8814,69 @@
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" style="21" customWidth="1"/>
     <col min="15" max="17" width="7.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" style="21" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" style="21" customWidth="1"/>
     <col min="20" max="21" width="10.140625" style="1" customWidth="1"/>
     <col min="22" max="22" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="125" t="s">
+      <c r="C1" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="128" t="s">
+      <c r="F1" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="129" t="s">
+      <c r="G1" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="130" t="s">
+      <c r="H1" s="128" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="132" t="s">
+      <c r="I1" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132" t="s">
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="133" t="s">
+      <c r="N1" s="130"/>
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="122" t="s">
+      <c r="R1" s="104" t="s">
         <v>144</v>
       </c>
-      <c r="S1" s="122"/>
+      <c r="S1" s="104"/>
       <c r="U1"/>
       <c r="V1"/>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="124"/>
-      <c r="B2" s="124"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="131"/>
+      <c r="A2" s="122"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="129"/>
       <c r="I2" s="16">
         <v>1</v>
       </c>
@@ -8853,14 +8898,14 @@
       <c r="O2" s="16">
         <v>3</v>
       </c>
-      <c r="P2" s="97" t="s">
+      <c r="P2" s="96" t="s">
         <v>137</v>
       </c>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="96" t="s">
-        <v>144</v>
-      </c>
-      <c r="S2" s="98" t="s">
+      <c r="Q2" s="132"/>
+      <c r="R2" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="S2" s="51" t="s">
         <v>50</v>
       </c>
     </row>
@@ -8890,10 +8935,10 @@
       <c r="A4" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="99" t="s">
+      <c r="B4" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="97" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="17"/>
@@ -8906,7 +8951,7 @@
       <c r="G4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="100" t="s">
+      <c r="H4" s="98" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="24" t="s">
@@ -8936,13 +8981,13 @@
       <c r="Q4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="101" t="s">
+      <c r="R4" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="S4" s="102" t="s">
+      <c r="S4" s="100" t="s">
         <v>143</v>
       </c>
-      <c r="V4" s="103" t="s">
+      <c r="V4" s="101" t="s">
         <v>139</v>
       </c>
     </row>
@@ -9289,7 +9334,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="79" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="74" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -9305,7 +9350,7 @@
   <dimension ref="A1:S97"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9322,65 +9367,65 @@
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" style="21" customWidth="1"/>
     <col min="15" max="17" width="7.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" style="21" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" style="21" customWidth="1"/>
     <col min="20" max="20" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="125" t="s">
+      <c r="C1" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="128" t="s">
+      <c r="F1" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="129" t="s">
+      <c r="G1" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="130" t="s">
+      <c r="H1" s="128" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="132" t="s">
+      <c r="I1" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132" t="s">
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="133" t="s">
+      <c r="N1" s="130"/>
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="122" t="s">
+      <c r="R1" s="104" t="s">
         <v>144</v>
       </c>
-      <c r="S1" s="122"/>
+      <c r="S1" s="104"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="124"/>
-      <c r="B2" s="124"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="131"/>
+      <c r="A2" s="122"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="129"/>
       <c r="I2" s="16">
         <v>1</v>
       </c>
@@ -9402,14 +9447,14 @@
       <c r="O2" s="16">
         <v>3</v>
       </c>
-      <c r="P2" s="97" t="s">
+      <c r="P2" s="96" t="s">
         <v>137</v>
       </c>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="96" t="s">
-        <v>144</v>
-      </c>
-      <c r="S2" s="98" t="s">
+      <c r="Q2" s="132"/>
+      <c r="R2" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="S2" s="51" t="s">
         <v>50</v>
       </c>
     </row>
@@ -9436,10 +9481,10 @@
       <c r="A4" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="99" t="s">
+      <c r="B4" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="97" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="17"/>
@@ -9452,7 +9497,7 @@
       <c r="G4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="100" t="s">
+      <c r="H4" s="98" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="24" t="s">
@@ -9482,10 +9527,10 @@
       <c r="Q4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="101" t="s">
+      <c r="R4" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="S4" s="102" t="s">
+      <c r="S4" s="100" t="s">
         <v>143</v>
       </c>
     </row>
@@ -9813,7 +9858,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="78" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="73" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -10070,7 +10115,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="76" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="71" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -10415,7 +10460,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="79" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="74" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>

</xml_diff>

<commit_message>
fixed headers for best lifter
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionBook/Scores-A4.xlsx
+++ b/owlcms/src/main/resources/templates/competitionBook/Scores-A4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8C82B7-8C47-448B-8DEB-31C44A84EE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C5A23F-366B-4D12-9780-BF55F434550F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="4065" windowWidth="23205" windowHeight="11295" tabRatio="447" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="447" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="35" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="149">
   <si>
     <t>${l.lastName}</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>${t.get("Category")}</t>
+  </si>
+  <si>
+    <t>${bestRankingTitle}</t>
   </si>
 </sst>
 </file>
@@ -6134,7 +6137,7 @@
   </sheetPr>
   <dimension ref="A1:Z107"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -8796,8 +8799,8 @@
   </sheetPr>
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8862,7 +8865,7 @@
         <v>48</v>
       </c>
       <c r="R1" s="104" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="S1" s="104"/>
       <c r="U1"/>
@@ -9326,7 +9329,7 @@
       <formula>AND(("$'Hommes Sinclair'.$#REF!$#REF!"),"$'Hommes Sinclair'.$#REF!$#REF!","$'Hommes Sinclair'.$#REF!$#REF!")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{F2F774F5-981E-458A-9101-9502A3FCC2A8}">
       <formula1>0</formula1>
       <formula2>200</formula2>
@@ -9350,7 +9353,7 @@
   <dimension ref="A1:S97"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="R1" sqref="R1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9413,7 +9416,7 @@
         <v>48</v>
       </c>
       <c r="R1" s="104" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="S1" s="104"/>
     </row>

</xml_diff>